<commit_message>
campo unidad para valores de factores
</commit_message>
<xml_diff>
--- a/back-end/Web Dinamico 2/MRVMinem/bin/Documentos/1.4 Plantilla_Auditoria_energetica.xlsx
+++ b/back-end/Web Dinamico 2/MRVMinem/bin/Documentos/1.4 Plantilla_Auditoria_energetica.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Web Dinamico 2\MRVMinem\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F5DB9-496A-4A56-8E10-53447B278DA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826725D6-2E64-4BBC-AB43-4A1251D1D896}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2E5039C4-2A71-47B3-941E-557D52B97803}"/>
   </bookViews>
@@ -35,18 +35,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>Anno</t>
   </si>
@@ -295,6 +289,9 @@
   </si>
   <si>
     <t xml:space="preserve">Fecha de implementación de la segunda auditoría y verificacion de resultadas estimadas del impacto. En caso se tenga que dejar vacia la celda, colocar la fecha (01/01/1920) Ingrese sus datos.  </t>
+  </si>
+  <si>
+    <t>Estado</t>
   </si>
 </sst>
 </file>
@@ -1371,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFC1772-35AF-4198-9510-18D55384E446}">
   <dimension ref="A1:AE316"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD10" sqref="AD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1500,7 @@
         <v>10</v>
       </c>
       <c r="AC2" s="62" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="AD2" s="63" t="s">
         <v>53</v>
@@ -23648,7 +23645,7 @@
       <c r="AD316" s="22"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="s1nrkz4hrZbHZq25fRmGJSSDVx/QOgyi81Nyio9AGgzwqteVYNsnK9bIk4xQQHjfkWv2aA3FvMwimKJAZQyBVw==" saltValue="Yh+zKwMRWCP5ydlnyI1ooA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZKfDqNtkYd0IWtR3yZ6D3IMqZtr/UdGyEnqU3kOG2Ph+HZ+tW7sC7/Sod5x6LV2aEWVokzOuX03H8suOVYvmcw==" saltValue="iTw+b6kLz0At8FUsGb7YBQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="6">
     <mergeCell ref="A3:AE3"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>